<commit_message>
add default taxonomy based on config
</commit_message>
<xml_diff>
--- a/data/combined_cleansed-SA Exercise.xlsx
+++ b/data/combined_cleansed-SA Exercise.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,30 +461,35 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Taxonomy</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Country</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>GBU</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>SAP ID</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Data Source</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Very Custom</t>
         </is>
@@ -514,24 +519,29 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>level 3</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>china</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Glass sourcing</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Glass Sourcing</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
         <v>2</v>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -557,24 +567,29 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>level 3</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>china</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Glass sourcing</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Glass Sourcing</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
         <v>5</v>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -600,24 +615,29 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t>level 3</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>spain</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Ingredient sourcing</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Ingredient Sourcing</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
         <v>7</v>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -643,24 +663,29 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>level 3</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>russia</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Ingredient sourcing</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Ingredient Sourcing</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
         <v>27</v>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -686,24 +711,29 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>level 3</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>spain</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Ingredient sourcing</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Ingredient Sourcing</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
         <v>81</v>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -729,24 +759,29 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
+          <t>level 3</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>spain</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Ingredient sourcing</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Ingredient Sourcing</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
         <v>45</v>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -772,28 +807,33 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
+          <t>level 3</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>france</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>Internal</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>Transport</t>
         </is>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>8</v>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>Transportation</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -823,28 +863,33 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t>level 3</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>indonesia</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>Internal</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>Transport</t>
         </is>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>12</v>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>Transportation</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -874,28 +919,33 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
+          <t>level 3</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>germany</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>Internal</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Use and end of life</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Use And End Of Life</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
         <v>6</v>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>Waste</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -925,28 +975,33 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>level 3</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>france</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>Internal</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Use and end of life</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Use And End Of Life</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
         <v>24</v>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>Waste</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>A</t>
         </is>

</xml_diff>

<commit_message>
add validation for ef config at end and rerun with new output
</commit_message>
<xml_diff>
--- a/data/combined_cleansed-SA Exercise.xlsx
+++ b/data/combined_cleansed-SA Exercise.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Taxonomy</t>
+          <t>EF ID CO2</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -471,25 +471,30 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>CO2AI Taxonomy</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>GBU</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>SAP ID</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Data Source</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Very Custom</t>
         </is>
@@ -517,10 +522,8 @@
       <c r="E2" t="n">
         <v>50</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>level 3</t>
-        </is>
+      <c r="F2" t="n">
+        <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -528,20 +531,21 @@
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Glass Sourcing</t>
-        </is>
-      </c>
-      <c r="J2" t="n">
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Glass sourcing</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
         <v>2</v>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -565,10 +569,8 @@
       <c r="E3" t="n">
         <v>50</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>level 3</t>
-        </is>
+      <c r="F3" t="n">
+        <v>2</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -576,20 +578,21 @@
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Glass Sourcing</t>
-        </is>
-      </c>
-      <c r="J3" t="n">
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Glass sourcing</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
         <v>5</v>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -613,31 +616,28 @@
       <c r="E4" t="n">
         <v>36</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>level 3</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
           <t>spain</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Ingredient Sourcing</t>
-        </is>
-      </c>
-      <c r="J4" t="n">
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Ingredient sourcing</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
         <v>7</v>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -661,31 +661,28 @@
       <c r="E5" t="n">
         <v>2857599</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>level 3</t>
-        </is>
-      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
           <t>russia</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Ingredient Sourcing</t>
-        </is>
-      </c>
-      <c r="J5" t="n">
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Ingredient sourcing</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
         <v>27</v>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -709,31 +706,28 @@
       <c r="E6" t="n">
         <v>2154562</v>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>level 3</t>
-        </is>
-      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
           <t>spain</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Ingredient Sourcing</t>
-        </is>
-      </c>
-      <c r="J6" t="n">
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Ingredient sourcing</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
         <v>81</v>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -757,31 +751,28 @@
       <c r="E7" t="n">
         <v>9500000</v>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>level 3</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
           <t>spain</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Ingredient Sourcing</t>
-        </is>
-      </c>
-      <c r="J7" t="n">
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Ingredient sourcing</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
         <v>45</v>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -805,11 +796,7 @@
       <c r="E8" t="n">
         <v>50</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>level 3</t>
-        </is>
-      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
           <t>france</t>
@@ -817,23 +804,28 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
+          <t>Transportation $ Goods transportation &amp; distribution $ Truck</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
           <t>Internal</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>Transport</t>
         </is>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>8</v>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>Transportation</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -861,11 +853,7 @@
       <c r="E9" t="n">
         <v>48280</v>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>level 3</t>
-        </is>
-      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
           <t>indonesia</t>
@@ -873,23 +861,28 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
+          <t>Transportation $ Goods transportation &amp; distribution $ Truck</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
           <t>Internal</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>Transport</t>
         </is>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>12</v>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>Transportation</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -917,11 +910,7 @@
       <c r="E10" t="n">
         <v>2000</v>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>level 3</t>
-        </is>
-      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
           <t>germany</t>
@@ -929,23 +918,28 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
+          <t>Use and end of life (waste) $ Waste treatment</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
           <t>Internal</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Use And End Of Life</t>
-        </is>
-      </c>
-      <c r="J10" t="n">
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Use and end of life</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
         <v>6</v>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>Waste</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -973,11 +967,7 @@
       <c r="E11" t="n">
         <v>45000000</v>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>level 3</t>
-        </is>
-      </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
           <t>france</t>
@@ -985,23 +975,28 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
+          <t>Use and end of life (waste) $ Waste treatment</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
           <t>Internal</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>Use And End Of Life</t>
-        </is>
-      </c>
-      <c r="J11" t="n">
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Use and end of life</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
         <v>24</v>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>Waste</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>A</t>
         </is>

</xml_diff>

<commit_message>
run etl with suppliers
</commit_message>
<xml_diff>
--- a/data/combined_cleansed-SA Exercise.xlsx
+++ b/data/combined_cleansed-SA Exercise.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,10 +491,15 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>Supplier Name</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>Data Source</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Very Custom</t>
         </is>
@@ -542,10 +547,15 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
+          <t>Glassy Glass inc.</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -589,10 +599,15 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
+          <t>Glassy Glass inc.</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -634,10 +649,15 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
+          <t>Spice girls inc.</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -679,10 +699,15 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
+          <t>Spice girls inc.</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -724,10 +749,15 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
+          <t>Spice girls inc.</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -769,10 +799,15 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
+          <t>Spice girls inc.</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -822,10 +857,15 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
+          <t>Ship happens inc.</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
           <t>Transportation</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -879,10 +919,15 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
+          <t>Ship happens inc.</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
           <t>Transportation</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -936,10 +981,15 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
+          <t>Dumpster Divers inc.</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
           <t>Waste</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -993,10 +1043,15 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
+          <t>Dumpster Divers inc.</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
           <t>Waste</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>A</t>
         </is>

</xml_diff>